<commit_message>
Commit con nuevos tokens
Science, SuchWow, new, dos puntos
</commit_message>
<xml_diff>
--- a/DC-AnalizadorLexico/Tokens.xlsx
+++ b/DC-AnalizadorLexico/Tokens.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Entero</t>
   </si>
@@ -154,13 +154,25 @@
   </si>
   <si>
     <t>"</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>science</t>
+  </si>
+  <si>
+    <t>SuchWow</t>
+  </si>
+  <si>
+    <t>:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,7 +271,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,7 +306,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -478,19 +490,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -507,7 +519,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -528,7 +540,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="18">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -549,7 +561,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="18">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -570,7 +582,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="18">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -591,7 +603,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="18">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -612,7 +624,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="18">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -633,7 +645,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="18">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -654,7 +666,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="18">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -675,7 +687,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="18">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -696,7 +708,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="18">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -717,7 +729,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="18">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -738,7 +750,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="18">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -759,7 +771,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="18">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -780,7 +792,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="18">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>14</v>
@@ -801,7 +813,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="18">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>15</v>
@@ -822,7 +834,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="18">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>16</v>
@@ -843,7 +855,7 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="18">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
         <v>20</v>
@@ -864,7 +876,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="18">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>17</v>
@@ -885,13 +897,13 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="18">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C20" s="1">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -906,13 +918,13 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="18">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -927,13 +939,13 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="18">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -948,13 +960,13 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="18">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -969,13 +981,13 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="18">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -990,13 +1002,13 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="18">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1011,13 +1023,13 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="18">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1032,13 +1044,13 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="18">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1053,13 +1065,13 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="18">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1074,13 +1086,13 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="18">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1095,132 +1107,177 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="18">
+      <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1">
+        <v>22</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" ht="18">
+      <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C31" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+    <row r="32" spans="1:15" ht="18">
+      <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C32" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
+    <row r="33" spans="2:3" ht="18">
+      <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C33" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
+    <row r="34" spans="2:3" ht="18">
+      <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C34" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
+    <row r="35" spans="2:3" ht="18">
+      <c r="B35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="18">
+      <c r="B36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C36" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
+    <row r="37" spans="2:3" ht="18">
+      <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C37" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+    <row r="38" spans="2:3" ht="18">
+      <c r="B38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C38" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
+    <row r="39" spans="2:3" ht="18">
+      <c r="B39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C39" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
+    <row r="40" spans="2:3" ht="18">
+      <c r="B40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C40" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
+    <row r="41" spans="2:3" ht="18">
+      <c r="B41" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C41" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
+    <row r="42" spans="2:3" ht="18">
+      <c r="B42" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C42" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+    <row r="43" spans="2:3" ht="18">
+      <c r="B43" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C43" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
+    <row r="44" spans="2:3" ht="18">
+      <c r="B44" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C44" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
+    <row r="45" spans="2:3" ht="18">
+      <c r="B45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C45" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
+    <row r="46" spans="2:3" ht="18">
+      <c r="B46" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C46" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
+    <row r="47" spans="2:3" ht="18">
+      <c r="B47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C47" s="1">
         <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="18">
+      <c r="B48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="18">
+      <c r="B49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="1">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>